<commit_message>
Fixed mistakes in formula (2.2) in lab 4.2.1. Finished work in lab 4.2.1. Renamed lab 4.2.1 to normal name.
Added 19_lab(task_3) in RC labs folder.
</commit_message>
<xml_diff>
--- a/Physics/4.2.1/4.2.1.xlsx
+++ b/Physics/4.2.1/4.2.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\4.2.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE650908-9FAD-4D89-8143-B7724E5A22F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C81F00A-FEF5-4BF9-9763-B227EBBDC80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{FED1618D-71A0-4FA6-A353-332A2123E11E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{FED1618D-71A0-4FA6-A353-332A2123E11E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -166,16 +166,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F52C94-8296-4D61-8C95-8CBE132361FC}">
-  <dimension ref="A2:O15"/>
+  <dimension ref="A2:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,16 +510,16 @@
   <sheetData>
     <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -576,11 +576,11 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -822,19 +822,19 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5">
-        <v>12</v>
+      <c r="C14" s="3">
+        <v>14</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="1">
-        <f>546/12</f>
-        <v>45.5</v>
+        <f>546/C14</f>
+        <v>39</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -863,6 +863,280 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <f>B4+C4/100</f>
+        <v>3.61</v>
+      </c>
+      <c r="C17">
+        <f>- (B17-3.61) * 0.1</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>C17*C17</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="C17:E17" si="0">E4+F4/100</f>
+        <v>2.84</v>
+      </c>
+      <c r="F17">
+        <f>- (E17-3.61) * 0.1</f>
+        <v>7.7000000000000013E-2</v>
+      </c>
+      <c r="G17">
+        <f>F17*F17</f>
+        <v>5.929000000000002E-3</v>
+      </c>
+      <c r="H17">
+        <f>G17-D18</f>
+        <v>-7.5269999999999938E-3</v>
+      </c>
+      <c r="J17">
+        <f>AVERAGE(H17:H22)</f>
+        <v>-7.6789999999999879E-3</v>
+      </c>
+      <c r="K17">
+        <f>-H17-$J$17</f>
+        <v>1.5205999999999982E-2</v>
+      </c>
+      <c r="L17">
+        <f>K17*K17</f>
+        <v>2.3122243599999945E-4</v>
+      </c>
+      <c r="M17">
+        <f>SUM(L17:L23)</f>
+        <v>1.4865463649999951E-3</v>
+      </c>
+      <c r="N17">
+        <f>SQRT(M17)</f>
+        <v>3.8555756574083659E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <f t="shared" ref="B18:B26" si="1">B5+C5/100</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C23" si="2">- (B18-3.61) * 0.1</f>
+        <v>0.11599999999999998</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:D23" si="3">C18*C18</f>
+        <v>1.3455999999999996E-2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18" si="4">E5+F5/100</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ref="F18:F23" si="5">- (E18-3.61) * 0.1</f>
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G23" si="6">F18*F18</f>
+        <v>2.0448999999999995E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H23" si="7">G18-D19</f>
+        <v>-7.4400000000000091E-3</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18:K23" si="8">-H18-$J$17</f>
+        <v>1.5118999999999997E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L23" si="9">K18*K18</f>
+        <v>2.2858416099999992E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>1.94</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>2.7889000000000004E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19" si="10">E6+F6/100</f>
+        <v>1.75</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>0.186</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="6"/>
+        <v>3.4596000000000002E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="7"/>
+        <v>-7.8399999999999789E-3</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="8"/>
+        <v>1.5518999999999967E-2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="9"/>
+        <v>2.4083936099999898E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>1.55</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>0.20599999999999996</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>4.2435999999999981E-2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20" si="11">E7+F7/100</f>
+        <v>1.38</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>0.223</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="6"/>
+        <v>4.9729000000000002E-2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="7"/>
+        <v>-5.4959999999999939E-3</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="8"/>
+        <v>1.3174999999999982E-2</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="9"/>
+        <v>1.7358062499999951E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>5.5224999999999996E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" si="12">E8+F8/100</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>-1.0399999999999979E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="8"/>
+        <v>1.8078999999999967E-2</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="9"/>
+        <v>3.2685024099999877E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>0.91</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>0.26999999999999996</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="3"/>
+        <v>7.2899999999999979E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22" si="13">E9+F9/100</f>
+        <v>0.84</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="6"/>
+        <v>7.6729000000000019E-2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="7"/>
+        <v>-7.3709999999999748E-3</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="8"/>
+        <v>1.5049999999999963E-2</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="9"/>
+        <v>2.2650249999999888E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>0.71</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="3"/>
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23" si="14">E10+F10/100</f>
+        <v>0.6</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="6"/>
+        <v>9.0600999999999987E-2</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="8"/>
+        <v>7.6789999999999879E-3</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="9"/>
+        <v>5.8967040999999816E-5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:D2"/>

</xml_diff>